<commit_message>
sorting out a problem with p12 curve-stripped data in preview/operations.py
</commit_message>
<xml_diff>
--- a/CATE Template - (2014_11_21).xlsx
+++ b/CATE Template - (2014_11_21).xlsx
@@ -50,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +65,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,10 +150,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -168,9 +174,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -471,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,8 +570,8 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
-        <v>81453</v>
+      <c r="C9" s="9">
+        <v>42489.7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,8 +581,8 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="3">
-        <v>20369.099999999999</v>
+      <c r="C10" s="9">
+        <v>12981.4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -584,8 +592,8 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="3">
-        <v>5511</v>
+      <c r="C11" s="9">
+        <v>4944.1000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,8 +603,8 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="3">
-        <v>2790.7</v>
+      <c r="C12" s="9">
+        <v>3005.1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,8 +614,8 @@
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="3">
-        <v>1933.8</v>
+      <c r="C13" s="9">
+        <v>1972.2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,8 +625,8 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="3">
-        <v>1456.8</v>
+      <c r="C14" s="9">
+        <v>1521.9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,8 +636,8 @@
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="3">
-        <v>1159.5</v>
+      <c r="C15" s="9">
+        <v>301.89999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,8 +647,8 @@
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="3">
-        <v>1015.1</v>
+      <c r="C16" s="9">
+        <v>1013.6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,8 +658,8 @@
       <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="3">
-        <v>882.4</v>
+      <c r="C17" s="9">
+        <v>828.6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,8 +669,8 @@
       <c r="B18" s="3">
         <v>10</v>
       </c>
-      <c r="C18" s="3">
-        <v>788.5</v>
+      <c r="C18" s="9">
+        <v>685.8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,8 +680,8 @@
       <c r="B19" s="3">
         <v>11.5</v>
       </c>
-      <c r="C19" s="3">
-        <v>801.7</v>
+      <c r="C19" s="9">
+        <v>532</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,8 +691,8 @@
       <c r="B20" s="3">
         <v>13</v>
       </c>
-      <c r="C20" s="3">
-        <v>698.5</v>
+      <c r="C20" s="9">
+        <v>503.7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,8 +702,8 @@
       <c r="B21" s="3">
         <v>14.5</v>
       </c>
-      <c r="C21" s="3">
-        <v>647.9</v>
+      <c r="C21" s="9">
+        <v>576.4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,8 +713,8 @@
       <c r="B22" s="3">
         <v>16</v>
       </c>
-      <c r="C22" s="3">
-        <v>629.29999999999995</v>
+      <c r="C22" s="9">
+        <v>421.6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,8 +724,8 @@
       <c r="B23" s="3">
         <v>17.5</v>
       </c>
-      <c r="C23" s="3">
-        <v>622.20000000000005</v>
+      <c r="C23" s="9">
+        <v>403</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,8 +735,8 @@
       <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C24" s="3">
-        <v>507.9</v>
+      <c r="C24" s="9">
+        <v>279.2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,8 +746,8 @@
       <c r="B25" s="3">
         <v>20.5</v>
       </c>
-      <c r="C25" s="3">
-        <v>504.2</v>
+      <c r="C25" s="9">
+        <v>221.6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -749,8 +757,8 @@
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="C26" s="3">
-        <v>422.8</v>
+      <c r="C26" s="9">
+        <v>245.6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,8 +768,8 @@
       <c r="B27" s="3">
         <v>23.5</v>
       </c>
-      <c r="C27" s="3">
-        <v>451.9</v>
+      <c r="C27" s="9">
+        <v>238.8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,8 +779,8 @@
       <c r="B28" s="3">
         <v>25</v>
       </c>
-      <c r="C28" s="3">
-        <v>411.3</v>
+      <c r="C28" s="9">
+        <v>225.8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -782,8 +790,8 @@
       <c r="B29" s="3">
         <v>27</v>
       </c>
-      <c r="C29" s="3">
-        <v>475.7</v>
+      <c r="C29" s="9">
+        <v>250.8</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,8 +801,8 @@
       <c r="B30" s="3">
         <v>29</v>
       </c>
-      <c r="C30" s="3">
-        <v>453.3</v>
+      <c r="C30" s="9">
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,8 +812,8 @@
       <c r="B31" s="3">
         <v>31</v>
       </c>
-      <c r="C31" s="3">
-        <v>467.4</v>
+      <c r="C31" s="9">
+        <v>220.4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -815,8 +823,8 @@
       <c r="B32" s="3">
         <v>33</v>
       </c>
-      <c r="C32" s="3">
-        <v>431.2</v>
+      <c r="C32" s="9">
+        <v>236.4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,8 +834,8 @@
       <c r="B33" s="3">
         <v>35</v>
       </c>
-      <c r="C33" s="3">
-        <v>404.4</v>
+      <c r="C33" s="9">
+        <v>214.7</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,8 +845,8 @@
       <c r="B34" s="3">
         <v>37</v>
       </c>
-      <c r="C34" s="3">
-        <v>432.2</v>
+      <c r="C34" s="9">
+        <v>190.1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,8 +856,8 @@
       <c r="B35" s="3">
         <v>39</v>
       </c>
-      <c r="C35" s="3">
-        <v>363.8</v>
+      <c r="C35" s="9">
+        <v>205.3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,8 +867,8 @@
       <c r="B36" s="3">
         <v>41</v>
       </c>
-      <c r="C36" s="3">
-        <v>429.8</v>
+      <c r="C36" s="9">
+        <v>210.8</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,8 +878,8 @@
       <c r="B37" s="3">
         <v>43</v>
       </c>
-      <c r="C37" s="3">
-        <v>303.39999999999998</v>
+      <c r="C37" s="9">
+        <v>145.5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,8 +889,8 @@
       <c r="B38" s="4">
         <v>45</v>
       </c>
-      <c r="C38" s="4">
-        <v>348.1</v>
+      <c r="C38" s="9">
+        <v>151.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
everything works, starting to create class that will direct flow of entire program
</commit_message>
<xml_diff>
--- a/CATE Template - (2014_11_21).xlsx
+++ b/CATE Template - (2014_11_21).xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Vial #</t>
   </si>
@@ -40,10 +40,13 @@
     <t>G-Factor</t>
   </si>
   <si>
-    <t>Run 1</t>
+    <t>Load Time (min)</t>
   </si>
   <si>
-    <t>Load Time (min)</t>
+    <t>Fucked</t>
+  </si>
+  <si>
+    <t>Run1</t>
   </si>
 </sst>
 </file>
@@ -98,21 +101,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -149,23 +137,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -175,6 +171,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,89 +482,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="2">
         <v>35714.845000000001</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2">
+        <v>17896.21</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2">
         <v>8679.2999999999993</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3">
+        <v>11535.5</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2">
         <v>4746.2</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4">
+        <v>3529.2000000000003</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2">
         <v>0.60270000000000001</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="9">
+        <v>0.88919999999999977</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2">
         <v>1.0084176343828599</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="10">
+        <v>1.0523687869528029</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="8"/>
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="2">
         <v>60</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="9">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -570,8 +589,11 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>42489.7</v>
+      </c>
+      <c r="D9" s="8">
+        <v>42177.599999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -581,8 +603,11 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>12981.4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>13410.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -592,8 +617,11 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>4944.1000000000004</v>
+      </c>
+      <c r="D11" s="8">
+        <v>4104.6000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -603,8 +631,11 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>3005.1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2033.4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,8 +645,11 @@
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>1972.2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1297</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,8 +659,11 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>1521.9</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1041</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,8 +673,11 @@
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>301.89999999999998</v>
+      </c>
+      <c r="D15" s="8">
+        <v>718.9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -647,250 +687,319 @@
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <v>1013.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="8">
+        <v>616.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
       <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>828.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="8">
+        <v>513.29999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>10</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>685.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="8">
+        <v>410.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11</v>
       </c>
       <c r="B19" s="3">
         <v>11.5</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>532</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="8">
+        <v>421.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
       <c r="B20" s="3">
         <v>13</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>503.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="8">
+        <v>429.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
       <c r="B21" s="3">
         <v>14.5</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <v>576.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="8">
+        <v>302.10000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
       <c r="B22" s="3">
         <v>16</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <v>421.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="8">
+        <v>320.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
       <c r="B23" s="3">
         <v>17.5</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>403</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="8">
+        <v>291.39999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
       <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>279.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="8">
+        <v>230.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>17</v>
       </c>
       <c r="B25" s="3">
         <v>20.5</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <v>221.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="8">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>18</v>
       </c>
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8">
         <v>245.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="8">
+        <v>194.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
       <c r="B27" s="3">
         <v>23.5</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <v>238.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="8">
+        <v>272.10000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20</v>
       </c>
       <c r="B28" s="3">
         <v>25</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>225.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="8">
+        <v>178.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>21</v>
       </c>
       <c r="B29" s="3">
         <v>27</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>250.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="8">
+        <v>183.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>22</v>
       </c>
       <c r="B30" s="3">
         <v>29</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <v>207</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="8">
+        <v>170.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
       <c r="B31" s="3">
         <v>31</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <v>220.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="8">
+        <v>178.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>24</v>
       </c>
       <c r="B32" s="3">
         <v>33</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>236.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="8">
+        <v>178.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>25</v>
       </c>
       <c r="B33" s="3">
         <v>35</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <v>214.7</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="8">
+        <v>163.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>26</v>
       </c>
       <c r="B34" s="3">
         <v>37</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <v>190.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="8">
+        <v>143.69999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>27</v>
       </c>
       <c r="B35" s="3">
         <v>39</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <v>205.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="8">
+        <v>149.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
       <c r="B36" s="3">
         <v>41</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <v>210.8</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="8">
+        <v>150.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
       <c r="B37" s="3">
         <v>43</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <v>145.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="8">
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>30</v>
       </c>
       <c r="B38" s="4">
         <v>45</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <v>151.9</v>
+      </c>
+      <c r="D38" s="8">
+        <v>88.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>